<commit_message>
Added a vector of meshes
</commit_message>
<xml_diff>
--- a/Tests_etc/Classes_calendar.xlsx
+++ b/Tests_etc/Classes_calendar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\z_FS\3111_3D\2022\INFO3111S22\Tests_etc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC87FD9A-F71B-4F8C-9945-FDFD11152BAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C34A2F8E-3F30-4CB4-95DD-E71BE8F4A443}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -135,9 +135,6 @@
     <t>Project #2 due</t>
   </si>
   <si>
-    <t>Friday, July 15th, 2022</t>
-  </si>
-  <si>
     <t>Checkpoint #1 due</t>
   </si>
   <si>
@@ -175,6 +172,9 @@
   </si>
   <si>
     <t>INFO-3111 "C++ Graphics" Summer 2022 : Professor Michael Feeney</t>
+  </si>
+  <si>
+    <t>Friday, July 22nd, 2022</t>
   </si>
 </sst>
 </file>
@@ -503,8 +503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -516,7 +516,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -535,7 +535,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -546,7 +546,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -557,7 +557,7 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -568,7 +568,7 @@
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
@@ -579,7 +579,7 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
@@ -590,7 +590,7 @@
         <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -601,7 +601,7 @@
         <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
@@ -614,7 +614,7 @@
         <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
@@ -633,7 +633,7 @@
         <v>23</v>
       </c>
       <c r="C19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
@@ -644,7 +644,7 @@
         <v>24</v>
       </c>
       <c r="C21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
@@ -655,7 +655,7 @@
         <v>25</v>
       </c>
       <c r="C22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
@@ -666,7 +666,7 @@
         <v>26</v>
       </c>
       <c r="C24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
@@ -677,7 +677,7 @@
         <v>27</v>
       </c>
       <c r="C25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Basic lighting on and checkpoint #6
</commit_message>
<xml_diff>
--- a/Tests_etc/Classes_calendar.xlsx
+++ b/Tests_etc/Classes_calendar.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\z_FS\3111_3D\2022\INFO3111S22\Tests_etc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29BE43F8-CAA9-4EED-803D-1C1103E7B5C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
+    <workbookView xWindow="2950" yWindow="480" windowWidth="12980" windowHeight="9400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -162,20 +168,20 @@
     <t>Checkpoint #11 due</t>
   </si>
   <si>
-    <t>Checkpoint #12 due</t>
-  </si>
-  <si>
     <t>INFO-3111 "C++ Graphics" Summer 2022 : Professor Michael Feeney</t>
   </si>
   <si>
     <t>Friday, July 22nd, 2022</t>
+  </si>
+  <si>
+    <t>**No checkpoint**</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -212,9 +218,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -249,7 +256,13 @@
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="7" name="Group 6"/>
+        <xdr:cNvPr id="7" name="Group 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGrpSpPr/>
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
@@ -262,7 +275,13 @@
       </xdr:grpSpPr>
       <xdr:cxnSp macro="">
         <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="3" name="Straight Connector 2"/>
+          <xdr:cNvPr id="3" name="Straight Connector 2">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvCxnSpPr/>
         </xdr:nvCxnSpPr>
         <xdr:spPr>
@@ -292,7 +311,13 @@
       </xdr:cxnSp>
       <xdr:cxnSp macro="">
         <xdr:nvCxnSpPr>
-          <xdr:cNvPr id="5" name="Straight Arrow Connector 4"/>
+          <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
           <xdr:cNvCxnSpPr/>
         </xdr:nvCxnSpPr>
         <xdr:spPr>
@@ -583,33 +608,33 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C13" sqref="C12:C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.453125" customWidth="1"/>
     <col min="2" max="2" width="25.26953125" customWidth="1"/>
     <col min="3" max="3" width="17.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -617,7 +642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -628,7 +653,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -639,7 +664,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -650,7 +675,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -661,7 +686,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -672,18 +697,18 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>20</v>
       </c>
-      <c r="C12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="C12" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -691,23 +716,23 @@
         <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -718,7 +743,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -726,10 +751,10 @@
         <v>23</v>
       </c>
       <c r="C19" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>15</v>
       </c>
@@ -737,10 +762,10 @@
         <v>24</v>
       </c>
       <c r="C21" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -748,10 +773,10 @@
         <v>25</v>
       </c>
       <c r="C22" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>17</v>
       </c>
@@ -759,10 +784,10 @@
         <v>26</v>
       </c>
       <c r="C24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>18</v>
       </c>
@@ -770,15 +795,15 @@
         <v>27</v>
       </c>
       <c r="C25" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>29</v>
       </c>
@@ -786,17 +811,17 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>32</v>
       </c>

</xml_diff>